<commit_message>
front legt and back right done
</commit_message>
<xml_diff>
--- a/servo_DEG-PWM.xlsx
+++ b/servo_DEG-PWM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlan\OneDrive\Desktop\2semestre\Bonzo - GoodBoy 0.0.0\botzo_v2s_github\botzo_servo_callibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5C59EC-6C21-41FF-95EF-15A37AB11563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3555656B-F88F-4E57-80F7-953CD19CFBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -417,11 +417,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -432,6 +427,11 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -657,8 +657,8 @@
   </sheetPr>
   <dimension ref="B5:K124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="59" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I82" sqref="I82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -782,13 +782,13 @@
       <c r="D39" s="12"/>
     </row>
     <row r="40" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="24" t="s">
+      <c r="B40" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="26"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="23"/>
       <c r="H40" s="9" t="s">
         <v>7</v>
       </c>
@@ -820,7 +820,7 @@
       </c>
     </row>
     <row r="42" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B42" s="27" t="s">
+      <c r="B42" s="24" t="s">
         <v>15</v>
       </c>
       <c r="C42" s="3">
@@ -836,18 +836,18 @@
         <f>E42-D42</f>
         <v>100</v>
       </c>
-      <c r="H42" s="21">
+      <c r="H42" s="27">
         <v>0</v>
       </c>
-      <c r="I42" s="21">
+      <c r="I42" s="27">
         <v>7.5270000000000001</v>
       </c>
-      <c r="J42" s="21">
+      <c r="J42" s="27">
         <v>597.6</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B43" s="28"/>
+      <c r="B43" s="25"/>
       <c r="C43" s="3">
         <v>45</v>
       </c>
@@ -861,12 +861,12 @@
         <f t="shared" ref="F43:F56" si="0">E43-D43</f>
         <v>100</v>
       </c>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="28"/>
     </row>
     <row r="44" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B44" s="28"/>
+      <c r="B44" s="25"/>
       <c r="C44" s="3">
         <v>90</v>
       </c>
@@ -880,12 +880,12 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="28"/>
     </row>
     <row r="45" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B45" s="28"/>
+      <c r="B45" s="25"/>
       <c r="C45" s="3">
         <v>135</v>
       </c>
@@ -899,12 +899,12 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
     </row>
     <row r="46" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="29"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="5">
         <v>180</v>
       </c>
@@ -918,12 +918,12 @@
         <f t="shared" si="0"/>
         <v>107</v>
       </c>
-      <c r="H46" s="23"/>
-      <c r="I46" s="23"/>
-      <c r="J46" s="23"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
     </row>
     <row r="47" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B47" s="27" t="s">
+      <c r="B47" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C47" s="3">
@@ -939,18 +939,18 @@
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="H47" s="21">
+      <c r="H47" s="27">
         <v>0</v>
       </c>
-      <c r="I47" s="21">
+      <c r="I47" s="27">
         <v>7.6820000000000004</v>
       </c>
-      <c r="J47" s="21">
+      <c r="J47" s="27">
         <v>578.14200000000005</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B48" s="28"/>
+      <c r="B48" s="25"/>
       <c r="C48" s="3">
         <v>45</v>
       </c>
@@ -964,12 +964,12 @@
         <f t="shared" si="0"/>
         <v>87</v>
       </c>
-      <c r="H48" s="22"/>
-      <c r="I48" s="22"/>
-      <c r="J48" s="22"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="28"/>
+      <c r="J48" s="28"/>
     </row>
     <row r="49" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B49" s="28"/>
+      <c r="B49" s="25"/>
       <c r="C49" s="3">
         <v>90</v>
       </c>
@@ -983,12 +983,12 @@
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="H49" s="22"/>
-      <c r="I49" s="22"/>
-      <c r="J49" s="22"/>
+      <c r="H49" s="28"/>
+      <c r="I49" s="28"/>
+      <c r="J49" s="28"/>
     </row>
     <row r="50" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B50" s="28"/>
+      <c r="B50" s="25"/>
       <c r="C50" s="3">
         <v>135</v>
       </c>
@@ -1002,12 +1002,12 @@
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
-      <c r="H50" s="22"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="28"/>
+      <c r="J50" s="28"/>
     </row>
     <row r="51" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="29"/>
+      <c r="B51" s="26"/>
       <c r="C51" s="5">
         <v>180</v>
       </c>
@@ -1021,12 +1021,12 @@
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="H51" s="23"/>
-      <c r="I51" s="23"/>
-      <c r="J51" s="23"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="29"/>
     </row>
     <row r="52" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B52" s="27" t="s">
+      <c r="B52" s="24" t="s">
         <v>17</v>
       </c>
       <c r="C52" s="3">
@@ -1042,18 +1042,18 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="H52" s="21">
+      <c r="H52" s="27">
         <v>0</v>
       </c>
-      <c r="I52" s="21">
+      <c r="I52" s="27">
         <v>7.3140000000000001</v>
       </c>
-      <c r="J52" s="21">
+      <c r="J52" s="27">
         <v>619.02800000000002</v>
       </c>
     </row>
     <row r="53" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B53" s="28"/>
+      <c r="B53" s="25"/>
       <c r="C53" s="3">
         <v>45</v>
       </c>
@@ -1067,12 +1067,12 @@
         <f t="shared" si="0"/>
         <v>117</v>
       </c>
-      <c r="H53" s="22"/>
-      <c r="I53" s="22"/>
-      <c r="J53" s="22"/>
+      <c r="H53" s="28"/>
+      <c r="I53" s="28"/>
+      <c r="J53" s="28"/>
     </row>
     <row r="54" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="28"/>
+      <c r="B54" s="25"/>
       <c r="C54" s="3">
         <v>90</v>
       </c>
@@ -1086,12 +1086,12 @@
         <f t="shared" si="0"/>
         <v>111</v>
       </c>
-      <c r="H54" s="22"/>
-      <c r="I54" s="22"/>
-      <c r="J54" s="22"/>
+      <c r="H54" s="28"/>
+      <c r="I54" s="28"/>
+      <c r="J54" s="28"/>
     </row>
     <row r="55" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B55" s="28"/>
+      <c r="B55" s="25"/>
       <c r="C55" s="3">
         <v>135</v>
       </c>
@@ -1105,12 +1105,12 @@
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
-      <c r="H55" s="22"/>
-      <c r="I55" s="22"/>
-      <c r="J55" s="22"/>
+      <c r="H55" s="28"/>
+      <c r="I55" s="28"/>
+      <c r="J55" s="28"/>
     </row>
     <row r="56" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="29"/>
+      <c r="B56" s="26"/>
       <c r="C56" s="5">
         <v>180</v>
       </c>
@@ -1124,9 +1124,9 @@
         <f t="shared" si="0"/>
         <v>127</v>
       </c>
-      <c r="H56" s="23"/>
-      <c r="I56" s="23"/>
-      <c r="J56" s="23"/>
+      <c r="H56" s="29"/>
+      <c r="I56" s="29"/>
+      <c r="J56" s="29"/>
     </row>
     <row r="57" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
       <c r="C57" s="12"/>
@@ -1192,7 +1192,7 @@
       </c>
     </row>
     <row r="65" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B65" s="27" t="s">
+      <c r="B65" s="24" t="s">
         <v>20</v>
       </c>
       <c r="C65" s="3">
@@ -1202,24 +1202,24 @@
         <v>500</v>
       </c>
       <c r="E65" s="3">
-        <v>570</v>
+        <v>640</v>
       </c>
       <c r="F65" s="13">
         <f>E65-D65</f>
-        <v>70</v>
-      </c>
-      <c r="H65" s="21">
+        <v>140</v>
+      </c>
+      <c r="H65" s="27">
         <v>0</v>
       </c>
-      <c r="I65" s="21">
+      <c r="I65" s="27">
         <v>7.274</v>
       </c>
-      <c r="J65" s="21">
+      <c r="J65" s="27">
         <v>569.57100000000003</v>
       </c>
     </row>
     <row r="66" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B66" s="28"/>
+      <c r="B66" s="25"/>
       <c r="C66" s="3">
         <v>45</v>
       </c>
@@ -1227,18 +1227,18 @@
         <v>833</v>
       </c>
       <c r="E66" s="3">
-        <v>900</v>
+        <v>980</v>
       </c>
       <c r="F66" s="13">
         <f t="shared" ref="F66:F79" si="1">E66-D66</f>
-        <v>67</v>
-      </c>
-      <c r="H66" s="22"/>
-      <c r="I66" s="22"/>
-      <c r="J66" s="22"/>
+        <v>147</v>
+      </c>
+      <c r="H66" s="28"/>
+      <c r="I66" s="28"/>
+      <c r="J66" s="28"/>
     </row>
     <row r="67" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B67" s="28"/>
+      <c r="B67" s="25"/>
       <c r="C67" s="3">
         <v>90</v>
       </c>
@@ -1246,18 +1246,18 @@
         <v>1167</v>
       </c>
       <c r="E67" s="3">
-        <v>1225</v>
+        <v>1320</v>
       </c>
       <c r="F67" s="13">
         <f t="shared" si="1"/>
-        <v>58</v>
-      </c>
-      <c r="H67" s="22"/>
-      <c r="I67" s="22"/>
-      <c r="J67" s="22"/>
+        <v>153</v>
+      </c>
+      <c r="H67" s="28"/>
+      <c r="I67" s="28"/>
+      <c r="J67" s="28"/>
     </row>
     <row r="68" spans="2:10" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B68" s="28"/>
+      <c r="B68" s="25"/>
       <c r="C68" s="3">
         <v>135</v>
       </c>
@@ -1265,18 +1265,18 @@
         <v>1500</v>
       </c>
       <c r="E68" s="3">
-        <v>1575</v>
+        <v>1670</v>
       </c>
       <c r="F68" s="13">
         <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-      <c r="H68" s="22"/>
-      <c r="I68" s="22"/>
-      <c r="J68" s="22"/>
+        <v>170</v>
+      </c>
+      <c r="H68" s="28"/>
+      <c r="I68" s="28"/>
+      <c r="J68" s="28"/>
     </row>
     <row r="69" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="29"/>
+      <c r="B69" s="26"/>
       <c r="C69" s="5">
         <v>180</v>
       </c>
@@ -1284,18 +1284,18 @@
         <v>1833</v>
       </c>
       <c r="E69" s="5">
-        <v>1905</v>
+        <v>1999</v>
       </c>
       <c r="F69" s="15">
         <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-      <c r="H69" s="23"/>
-      <c r="I69" s="23"/>
-      <c r="J69" s="23"/>
+        <v>166</v>
+      </c>
+      <c r="H69" s="29"/>
+      <c r="I69" s="29"/>
+      <c r="J69" s="29"/>
     </row>
     <row r="70" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="27" t="s">
+      <c r="B70" s="24" t="s">
         <v>21</v>
       </c>
       <c r="C70" s="3">
@@ -1311,18 +1311,18 @@
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="H70" s="21">
+      <c r="H70" s="27">
         <v>0</v>
       </c>
-      <c r="I70" s="21">
+      <c r="I70" s="27">
         <v>7.6029999999999998</v>
       </c>
-      <c r="J70" s="21">
+      <c r="J70" s="27">
         <v>625.428</v>
       </c>
     </row>
     <row r="71" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="28"/>
+      <c r="B71" s="25"/>
       <c r="C71" s="3">
         <v>45</v>
       </c>
@@ -1336,12 +1336,12 @@
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
-      <c r="H71" s="22"/>
-      <c r="I71" s="22"/>
-      <c r="J71" s="22"/>
+      <c r="H71" s="28"/>
+      <c r="I71" s="28"/>
+      <c r="J71" s="28"/>
     </row>
     <row r="72" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="28"/>
+      <c r="B72" s="25"/>
       <c r="C72" s="3">
         <v>90</v>
       </c>
@@ -1355,12 +1355,12 @@
         <f t="shared" si="1"/>
         <v>143</v>
       </c>
-      <c r="H72" s="22"/>
-      <c r="I72" s="22"/>
-      <c r="J72" s="22"/>
+      <c r="H72" s="28"/>
+      <c r="I72" s="28"/>
+      <c r="J72" s="28"/>
     </row>
     <row r="73" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="28"/>
+      <c r="B73" s="25"/>
       <c r="C73" s="3">
         <v>135</v>
       </c>
@@ -1374,12 +1374,12 @@
         <f t="shared" si="1"/>
         <v>170</v>
       </c>
-      <c r="H73" s="22"/>
-      <c r="I73" s="22"/>
-      <c r="J73" s="22"/>
+      <c r="H73" s="28"/>
+      <c r="I73" s="28"/>
+      <c r="J73" s="28"/>
     </row>
     <row r="74" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="29"/>
+      <c r="B74" s="26"/>
       <c r="C74" s="5">
         <v>180</v>
       </c>
@@ -1393,12 +1393,12 @@
         <f t="shared" si="1"/>
         <v>167</v>
       </c>
-      <c r="H74" s="23"/>
-      <c r="I74" s="23"/>
-      <c r="J74" s="23"/>
+      <c r="H74" s="29"/>
+      <c r="I74" s="29"/>
+      <c r="J74" s="29"/>
     </row>
     <row r="75" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="27" t="s">
+      <c r="B75" s="24" t="s">
         <v>22</v>
       </c>
       <c r="C75" s="3">
@@ -1414,18 +1414,18 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="H75" s="21">
+      <c r="H75" s="27">
         <v>1E-3</v>
       </c>
-      <c r="I75" s="21">
+      <c r="I75" s="27">
         <v>7.2329999999999997</v>
       </c>
-      <c r="J75" s="21">
+      <c r="J75" s="27">
         <v>549.99900000000002</v>
       </c>
     </row>
     <row r="76" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="28"/>
+      <c r="B76" s="25"/>
       <c r="C76" s="3">
         <v>45</v>
       </c>
@@ -1439,12 +1439,12 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="H76" s="22"/>
-      <c r="I76" s="22"/>
-      <c r="J76" s="22"/>
+      <c r="H76" s="28"/>
+      <c r="I76" s="28"/>
+      <c r="J76" s="28"/>
     </row>
     <row r="77" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="28"/>
+      <c r="B77" s="25"/>
       <c r="C77" s="3">
         <v>90</v>
       </c>
@@ -1458,12 +1458,12 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="H77" s="22"/>
-      <c r="I77" s="22"/>
-      <c r="J77" s="22"/>
+      <c r="H77" s="28"/>
+      <c r="I77" s="28"/>
+      <c r="J77" s="28"/>
     </row>
     <row r="78" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="28"/>
+      <c r="B78" s="25"/>
       <c r="C78" s="3">
         <v>135</v>
       </c>
@@ -1477,12 +1477,12 @@
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="H78" s="22"/>
-      <c r="I78" s="22"/>
-      <c r="J78" s="22"/>
+      <c r="H78" s="28"/>
+      <c r="I78" s="28"/>
+      <c r="J78" s="28"/>
     </row>
     <row r="79" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="29"/>
+      <c r="B79" s="26"/>
       <c r="C79" s="5">
         <v>180</v>
       </c>
@@ -1496,22 +1496,22 @@
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="H79" s="23"/>
-      <c r="I79" s="23"/>
-      <c r="J79" s="23"/>
+      <c r="H79" s="29"/>
+      <c r="I79" s="29"/>
+      <c r="J79" s="29"/>
     </row>
     <row r="80" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F80" s="17"/>
     </row>
     <row r="84" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="24" t="s">
+      <c r="B85" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C85" s="25"/>
-      <c r="D85" s="25"/>
-      <c r="E85" s="25"/>
-      <c r="F85" s="26"/>
+      <c r="C85" s="31"/>
+      <c r="D85" s="31"/>
+      <c r="E85" s="31"/>
+      <c r="F85" s="32"/>
       <c r="H85" s="9" t="s">
         <v>7</v>
       </c>
@@ -1543,7 +1543,7 @@
       </c>
     </row>
     <row r="87" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="27" t="s">
+      <c r="B87" s="24" t="s">
         <v>24</v>
       </c>
       <c r="C87" s="3">
@@ -1553,24 +1553,24 @@
         <v>500</v>
       </c>
       <c r="E87" s="3">
-        <v>590</v>
+        <v>630</v>
       </c>
       <c r="F87" s="13">
         <f>E87-D87</f>
-        <v>90</v>
-      </c>
-      <c r="H87" s="21">
-        <v>1E-3</v>
-      </c>
-      <c r="I87" s="21">
-        <v>7.3869999999999996</v>
-      </c>
-      <c r="J87" s="21">
-        <v>584.28499999999997</v>
+        <v>130</v>
+      </c>
+      <c r="H87" s="27">
+        <v>0</v>
+      </c>
+      <c r="I87" s="27">
+        <v>7.5140000000000002</v>
+      </c>
+      <c r="J87" s="27">
+        <v>626.428</v>
       </c>
     </row>
     <row r="88" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="28"/>
+      <c r="B88" s="25"/>
       <c r="C88" s="3">
         <v>45</v>
       </c>
@@ -1578,18 +1578,18 @@
         <v>833</v>
       </c>
       <c r="E88" s="3">
-        <v>910</v>
+        <v>960</v>
       </c>
       <c r="F88" s="13">
         <f t="shared" ref="F88:F101" si="2">E88-D88</f>
-        <v>77</v>
-      </c>
-      <c r="H88" s="22"/>
-      <c r="I88" s="22"/>
-      <c r="J88" s="22"/>
+        <v>127</v>
+      </c>
+      <c r="H88" s="28"/>
+      <c r="I88" s="28"/>
+      <c r="J88" s="28"/>
     </row>
     <row r="89" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="28"/>
+      <c r="B89" s="25"/>
       <c r="C89" s="3">
         <v>90</v>
       </c>
@@ -1597,18 +1597,18 @@
         <v>1167</v>
       </c>
       <c r="E89" s="3">
-        <v>1250</v>
+        <v>1300</v>
       </c>
       <c r="F89" s="13">
         <f t="shared" si="2"/>
-        <v>83</v>
-      </c>
-      <c r="H89" s="22"/>
-      <c r="I89" s="22"/>
-      <c r="J89" s="22"/>
+        <v>133</v>
+      </c>
+      <c r="H89" s="28"/>
+      <c r="I89" s="28"/>
+      <c r="J89" s="28"/>
     </row>
     <row r="90" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="28"/>
+      <c r="B90" s="25"/>
       <c r="C90" s="3">
         <v>135</v>
       </c>
@@ -1616,18 +1616,18 @@
         <v>1500</v>
       </c>
       <c r="E90" s="3">
-        <v>1620</v>
+        <v>1660</v>
       </c>
       <c r="F90" s="13">
         <f t="shared" si="2"/>
-        <v>120</v>
-      </c>
-      <c r="H90" s="22"/>
-      <c r="I90" s="22"/>
-      <c r="J90" s="22"/>
+        <v>160</v>
+      </c>
+      <c r="H90" s="28"/>
+      <c r="I90" s="28"/>
+      <c r="J90" s="28"/>
     </row>
     <row r="91" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="29"/>
+      <c r="B91" s="26"/>
       <c r="C91" s="5">
         <v>180</v>
       </c>
@@ -1635,18 +1635,18 @@
         <v>1833</v>
       </c>
       <c r="E91" s="5">
-        <v>1940</v>
+        <v>1985</v>
       </c>
       <c r="F91" s="15">
         <f t="shared" si="2"/>
-        <v>107</v>
-      </c>
-      <c r="H91" s="23"/>
-      <c r="I91" s="23"/>
-      <c r="J91" s="23"/>
+        <v>152</v>
+      </c>
+      <c r="H91" s="29"/>
+      <c r="I91" s="29"/>
+      <c r="J91" s="29"/>
     </row>
     <row r="92" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="27" t="s">
+      <c r="B92" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C92" s="3">
@@ -1662,18 +1662,18 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="H92" s="21">
+      <c r="H92" s="27">
         <v>1E-3</v>
       </c>
-      <c r="I92" s="21">
+      <c r="I92" s="27">
         <v>7.3639999999999999</v>
       </c>
-      <c r="J92" s="21">
+      <c r="J92" s="27">
         <v>548.74199999999996</v>
       </c>
     </row>
     <row r="93" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="28"/>
+      <c r="B93" s="25"/>
       <c r="C93" s="3">
         <v>45</v>
       </c>
@@ -1687,12 +1687,12 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="H93" s="22"/>
-      <c r="I93" s="22"/>
-      <c r="J93" s="22"/>
+      <c r="H93" s="28"/>
+      <c r="I93" s="28"/>
+      <c r="J93" s="28"/>
     </row>
     <row r="94" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="28"/>
+      <c r="B94" s="25"/>
       <c r="C94" s="3">
         <v>90</v>
       </c>
@@ -1706,12 +1706,12 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="H94" s="22"/>
-      <c r="I94" s="22"/>
-      <c r="J94" s="22"/>
+      <c r="H94" s="28"/>
+      <c r="I94" s="28"/>
+      <c r="J94" s="28"/>
     </row>
     <row r="95" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="28"/>
+      <c r="B95" s="25"/>
       <c r="C95" s="3">
         <v>135</v>
       </c>
@@ -1725,12 +1725,12 @@
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="H95" s="22"/>
-      <c r="I95" s="22"/>
-      <c r="J95" s="22"/>
+      <c r="H95" s="28"/>
+      <c r="I95" s="28"/>
+      <c r="J95" s="28"/>
     </row>
     <row r="96" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="29"/>
+      <c r="B96" s="26"/>
       <c r="C96" s="5">
         <v>180</v>
       </c>
@@ -1744,12 +1744,12 @@
         <f t="shared" si="2"/>
         <v>87</v>
       </c>
-      <c r="H96" s="23"/>
-      <c r="I96" s="23"/>
-      <c r="J96" s="23"/>
+      <c r="H96" s="29"/>
+      <c r="I96" s="29"/>
+      <c r="J96" s="29"/>
     </row>
     <row r="97" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="27" t="s">
+      <c r="B97" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C97" s="3">
@@ -1765,18 +1765,18 @@
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="H97" s="21">
+      <c r="H97" s="27">
         <v>1E-3</v>
       </c>
-      <c r="I97" s="21">
+      <c r="I97" s="27">
         <v>7.1369999999999996</v>
       </c>
-      <c r="J97" s="21">
+      <c r="J97" s="27">
         <v>559.20000000000005</v>
       </c>
     </row>
     <row r="98" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="28"/>
+      <c r="B98" s="25"/>
       <c r="C98" s="3">
         <v>45</v>
       </c>
@@ -1790,12 +1790,12 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="H98" s="22"/>
-      <c r="I98" s="22"/>
-      <c r="J98" s="22"/>
+      <c r="H98" s="28"/>
+      <c r="I98" s="28"/>
+      <c r="J98" s="28"/>
     </row>
     <row r="99" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="28"/>
+      <c r="B99" s="25"/>
       <c r="C99" s="3">
         <v>90</v>
       </c>
@@ -1809,12 +1809,12 @@
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="H99" s="22"/>
-      <c r="I99" s="22"/>
-      <c r="J99" s="22"/>
+      <c r="H99" s="28"/>
+      <c r="I99" s="28"/>
+      <c r="J99" s="28"/>
     </row>
     <row r="100" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="28"/>
+      <c r="B100" s="25"/>
       <c r="C100" s="3">
         <v>135</v>
       </c>
@@ -1828,12 +1828,12 @@
         <f t="shared" si="2"/>
         <v>55</v>
       </c>
-      <c r="H100" s="22"/>
-      <c r="I100" s="22"/>
-      <c r="J100" s="22"/>
+      <c r="H100" s="28"/>
+      <c r="I100" s="28"/>
+      <c r="J100" s="28"/>
     </row>
     <row r="101" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="29"/>
+      <c r="B101" s="26"/>
       <c r="C101" s="5">
         <v>180</v>
       </c>
@@ -1847,22 +1847,22 @@
         <f t="shared" si="2"/>
         <v>57</v>
       </c>
-      <c r="H101" s="23"/>
-      <c r="I101" s="23"/>
-      <c r="J101" s="23"/>
+      <c r="H101" s="29"/>
+      <c r="I101" s="29"/>
+      <c r="J101" s="29"/>
     </row>
     <row r="102" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F102" s="17"/>
     </row>
     <row r="106" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="107" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B107" s="24" t="s">
+      <c r="B107" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C107" s="25"/>
-      <c r="D107" s="25"/>
-      <c r="E107" s="25"/>
-      <c r="F107" s="26"/>
+      <c r="C107" s="22"/>
+      <c r="D107" s="22"/>
+      <c r="E107" s="22"/>
+      <c r="F107" s="23"/>
       <c r="H107" s="9" t="s">
         <v>7</v>
       </c>
@@ -1894,7 +1894,7 @@
       </c>
     </row>
     <row r="109" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="27" t="s">
+      <c r="B109" s="24" t="s">
         <v>27</v>
       </c>
       <c r="C109" s="3">
@@ -1910,18 +1910,18 @@
         <f>E109-D109</f>
         <v>120</v>
       </c>
-      <c r="H109" s="21">
+      <c r="H109" s="27">
         <v>0</v>
       </c>
-      <c r="I109" s="21">
+      <c r="I109" s="27">
         <v>7.3840000000000003</v>
       </c>
-      <c r="J109" s="21">
+      <c r="J109" s="27">
         <v>614.85699999999997</v>
       </c>
     </row>
     <row r="110" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="28"/>
+      <c r="B110" s="25"/>
       <c r="C110" s="3">
         <v>45</v>
       </c>
@@ -1935,12 +1935,12 @@
         <f t="shared" ref="F110:F123" si="3">E110-D110</f>
         <v>107</v>
       </c>
-      <c r="H110" s="22"/>
-      <c r="I110" s="22"/>
-      <c r="J110" s="22"/>
+      <c r="H110" s="28"/>
+      <c r="I110" s="28"/>
+      <c r="J110" s="28"/>
     </row>
     <row r="111" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="28"/>
+      <c r="B111" s="25"/>
       <c r="C111" s="3">
         <v>90</v>
       </c>
@@ -1954,12 +1954,12 @@
         <f t="shared" si="3"/>
         <v>113</v>
       </c>
-      <c r="H111" s="22"/>
-      <c r="I111" s="22"/>
-      <c r="J111" s="22"/>
+      <c r="H111" s="28"/>
+      <c r="I111" s="28"/>
+      <c r="J111" s="28"/>
     </row>
     <row r="112" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="28"/>
+      <c r="B112" s="25"/>
       <c r="C112" s="3">
         <v>135</v>
       </c>
@@ -1973,12 +1973,12 @@
         <f t="shared" si="3"/>
         <v>140</v>
       </c>
-      <c r="H112" s="22"/>
-      <c r="I112" s="22"/>
-      <c r="J112" s="22"/>
+      <c r="H112" s="28"/>
+      <c r="I112" s="28"/>
+      <c r="J112" s="28"/>
     </row>
     <row r="113" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="29"/>
+      <c r="B113" s="26"/>
       <c r="C113" s="5">
         <v>180</v>
       </c>
@@ -1992,12 +1992,12 @@
         <f t="shared" si="3"/>
         <v>127</v>
       </c>
-      <c r="H113" s="23"/>
-      <c r="I113" s="23"/>
-      <c r="J113" s="23"/>
+      <c r="H113" s="29"/>
+      <c r="I113" s="29"/>
+      <c r="J113" s="29"/>
     </row>
     <row r="114" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="27" t="s">
+      <c r="B114" s="24" t="s">
         <v>29</v>
       </c>
       <c r="C114" s="3">
@@ -2013,18 +2013,18 @@
         <f t="shared" si="3"/>
         <v>130</v>
       </c>
-      <c r="H114" s="21">
+      <c r="H114" s="27">
         <v>0</v>
       </c>
-      <c r="I114" s="21">
+      <c r="I114" s="27">
         <v>7.7039999999999997</v>
       </c>
-      <c r="J114" s="21">
+      <c r="J114" s="27">
         <v>628.14200000000005</v>
       </c>
     </row>
     <row r="115" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="28"/>
+      <c r="B115" s="25"/>
       <c r="C115" s="3">
         <v>45</v>
       </c>
@@ -2038,12 +2038,12 @@
         <f t="shared" si="3"/>
         <v>137</v>
       </c>
-      <c r="H115" s="22"/>
-      <c r="I115" s="22"/>
-      <c r="J115" s="22"/>
+      <c r="H115" s="28"/>
+      <c r="I115" s="28"/>
+      <c r="J115" s="28"/>
     </row>
     <row r="116" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="28"/>
+      <c r="B116" s="25"/>
       <c r="C116" s="3">
         <v>90</v>
       </c>
@@ -2057,12 +2057,12 @@
         <f t="shared" si="3"/>
         <v>148</v>
       </c>
-      <c r="H116" s="22"/>
-      <c r="I116" s="22"/>
-      <c r="J116" s="22"/>
+      <c r="H116" s="28"/>
+      <c r="I116" s="28"/>
+      <c r="J116" s="28"/>
     </row>
     <row r="117" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="28"/>
+      <c r="B117" s="25"/>
       <c r="C117" s="3">
         <v>135</v>
       </c>
@@ -2076,12 +2076,12 @@
         <f t="shared" si="3"/>
         <v>160</v>
       </c>
-      <c r="H117" s="22"/>
-      <c r="I117" s="22"/>
-      <c r="J117" s="22"/>
+      <c r="H117" s="28"/>
+      <c r="I117" s="28"/>
+      <c r="J117" s="28"/>
     </row>
     <row r="118" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="29"/>
+      <c r="B118" s="26"/>
       <c r="C118" s="5">
         <v>180</v>
       </c>
@@ -2095,12 +2095,12 @@
         <f t="shared" si="3"/>
         <v>157</v>
       </c>
-      <c r="H118" s="23"/>
-      <c r="I118" s="23"/>
-      <c r="J118" s="23"/>
+      <c r="H118" s="29"/>
+      <c r="I118" s="29"/>
+      <c r="J118" s="29"/>
     </row>
     <row r="119" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="27" t="s">
+      <c r="B119" s="24" t="s">
         <v>30</v>
       </c>
       <c r="C119" s="3">
@@ -2116,18 +2116,18 @@
         <f t="shared" si="3"/>
         <v>140</v>
       </c>
-      <c r="H119" s="21">
+      <c r="H119" s="27">
         <v>-1E-3</v>
       </c>
-      <c r="I119" s="21">
+      <c r="I119" s="27">
         <v>7.7649999999999997</v>
       </c>
-      <c r="J119" s="21">
+      <c r="J119" s="27">
         <v>634.28499999999997</v>
       </c>
     </row>
     <row r="120" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="28"/>
+      <c r="B120" s="25"/>
       <c r="C120" s="3">
         <v>45</v>
       </c>
@@ -2141,12 +2141,12 @@
         <f t="shared" si="3"/>
         <v>137</v>
       </c>
-      <c r="H120" s="22"/>
-      <c r="I120" s="22"/>
-      <c r="J120" s="22"/>
+      <c r="H120" s="28"/>
+      <c r="I120" s="28"/>
+      <c r="J120" s="28"/>
     </row>
     <row r="121" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="28"/>
+      <c r="B121" s="25"/>
       <c r="C121" s="3">
         <v>90</v>
       </c>
@@ -2160,12 +2160,12 @@
         <f t="shared" si="3"/>
         <v>153</v>
       </c>
-      <c r="H121" s="22"/>
-      <c r="I121" s="22"/>
-      <c r="J121" s="22"/>
+      <c r="H121" s="28"/>
+      <c r="I121" s="28"/>
+      <c r="J121" s="28"/>
     </row>
     <row r="122" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="28"/>
+      <c r="B122" s="25"/>
       <c r="C122" s="3">
         <v>135</v>
       </c>
@@ -2179,12 +2179,12 @@
         <f t="shared" si="3"/>
         <v>170</v>
       </c>
-      <c r="H122" s="22"/>
-      <c r="I122" s="22"/>
-      <c r="J122" s="22"/>
+      <c r="H122" s="28"/>
+      <c r="I122" s="28"/>
+      <c r="J122" s="28"/>
     </row>
     <row r="123" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="29"/>
+      <c r="B123" s="26"/>
       <c r="C123" s="5">
         <v>180</v>
       </c>
@@ -2198,15 +2198,16 @@
         <f t="shared" si="3"/>
         <v>147</v>
       </c>
-      <c r="H123" s="23"/>
-      <c r="I123" s="23"/>
-      <c r="J123" s="23"/>
+      <c r="H123" s="29"/>
+      <c r="I123" s="29"/>
+      <c r="J123" s="29"/>
     </row>
     <row r="124" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F124" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B107:F107"/>
     <mergeCell ref="B119:B123"/>
     <mergeCell ref="H119:H123"/>
     <mergeCell ref="I119:I123"/>
@@ -2219,48 +2220,47 @@
     <mergeCell ref="H114:H118"/>
     <mergeCell ref="I114:I118"/>
     <mergeCell ref="J114:J118"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="H92:H96"/>
+    <mergeCell ref="I92:I96"/>
+    <mergeCell ref="J92:J96"/>
     <mergeCell ref="B97:B101"/>
     <mergeCell ref="H97:H101"/>
     <mergeCell ref="I97:I101"/>
     <mergeCell ref="J97:J101"/>
-    <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B85:F85"/>
     <mergeCell ref="B87:B91"/>
     <mergeCell ref="H87:H91"/>
     <mergeCell ref="I87:I91"/>
     <mergeCell ref="J87:J91"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="H92:H96"/>
-    <mergeCell ref="I92:I96"/>
-    <mergeCell ref="J92:J96"/>
+    <mergeCell ref="B70:B74"/>
+    <mergeCell ref="H70:H74"/>
+    <mergeCell ref="I70:I74"/>
+    <mergeCell ref="J70:J74"/>
     <mergeCell ref="B75:B79"/>
     <mergeCell ref="H75:H79"/>
     <mergeCell ref="I75:I79"/>
     <mergeCell ref="J75:J79"/>
-    <mergeCell ref="B85:F85"/>
+    <mergeCell ref="B63:F63"/>
     <mergeCell ref="B65:B69"/>
     <mergeCell ref="H65:H69"/>
     <mergeCell ref="I65:I69"/>
     <mergeCell ref="J65:J69"/>
-    <mergeCell ref="B70:B74"/>
-    <mergeCell ref="H70:H74"/>
-    <mergeCell ref="I70:I74"/>
-    <mergeCell ref="J70:J74"/>
+    <mergeCell ref="B47:B51"/>
+    <mergeCell ref="H47:H51"/>
+    <mergeCell ref="I47:I51"/>
+    <mergeCell ref="J47:J51"/>
     <mergeCell ref="B52:B56"/>
     <mergeCell ref="H52:H56"/>
     <mergeCell ref="I52:I56"/>
     <mergeCell ref="J52:J56"/>
-    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H14:I15"/>
+    <mergeCell ref="B40:F40"/>
     <mergeCell ref="B42:B46"/>
     <mergeCell ref="H42:H46"/>
     <mergeCell ref="I42:I46"/>
     <mergeCell ref="J42:J46"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="H47:H51"/>
-    <mergeCell ref="I47:I51"/>
-    <mergeCell ref="J47:J51"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H14:I15"/>
-    <mergeCell ref="B40:F40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>